<commit_message>
Fixed issue with two parallel starting operations and added Scheduling_ERT
</commit_message>
<xml_diff>
--- a/data/Operations_Data_Testing.xlsx
+++ b/data/Operations_Data_Testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\MSTS_FJSP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD938720-604C-411E-8FB6-C4BBF43F2DD3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54090E30-17CA-46F8-924F-CE1B5DE997DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{1D379F6F-46A7-404F-89DA-62600F8E0E9F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{1D379F6F-46A7-404F-89DA-62600F8E0E9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="46">
   <si>
     <t>Job</t>
   </si>
@@ -109,9 +109,6 @@
     <t>P2</t>
   </si>
   <si>
-    <t>P1</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
@@ -167,6 +164,36 @@
   </si>
   <si>
     <t>Finish_time</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>O31</t>
+  </si>
+  <si>
+    <t>O32</t>
+  </si>
+  <si>
+    <t>O33</t>
+  </si>
+  <si>
+    <t>O34</t>
+  </si>
+  <si>
+    <t>Boring</t>
+  </si>
+  <si>
+    <t>O31,O32</t>
+  </si>
+  <si>
+    <t>O35</t>
+  </si>
+  <si>
+    <t>Grooving</t>
+  </si>
+  <si>
+    <t>O34,O35</t>
   </si>
 </sst>
 </file>
@@ -524,7 +551,7 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -570,22 +597,22 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" t="s">
         <v>31</v>
-      </c>
-      <c r="L1" t="s">
-        <v>32</v>
       </c>
       <c r="M1" t="s">
         <v>9</v>
       </c>
       <c r="N1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
@@ -596,7 +623,7 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1">
         <v>3</v>
@@ -627,7 +654,7 @@
         <v>12</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N2" s="3"/>
       <c r="O2">
@@ -642,7 +669,7 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1">
         <v>5</v>
@@ -665,17 +692,17 @@
         <v>250</v>
       </c>
       <c r="J3" s="2">
-        <f t="shared" ref="J3:J11" si="1">H3+I3</f>
+        <f t="shared" ref="J3:J16" si="1">H3+I3</f>
         <v>920</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N3" s="3"/>
       <c r="O3">
@@ -690,7 +717,7 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
@@ -738,7 +765,7 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1">
         <v>2.5</v>
@@ -768,7 +795,7 @@
         <v>12</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>16</v>
@@ -786,7 +813,7 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" s="1">
         <v>50</v>
@@ -816,7 +843,7 @@
         <v>13</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>17</v>
@@ -831,10 +858,10 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" s="1">
         <v>4</v>
@@ -861,11 +888,11 @@
         <v>140</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N7" s="3"/>
       <c r="O7">
@@ -874,13 +901,13 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1">
         <v>2.5</v>
@@ -908,10 +935,10 @@
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N8" s="3"/>
       <c r="O8">
@@ -920,13 +947,13 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1">
         <v>2.35</v>
@@ -953,10 +980,10 @@
         <v>690</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>17</v>
@@ -968,13 +995,13 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="1">
         <v>23</v>
@@ -1001,10 +1028,10 @@
         <v>580</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>16</v>
@@ -1016,13 +1043,13 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" s="1">
         <v>5</v>
@@ -1049,11 +1076,11 @@
         <v>450</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N11" s="3"/>
       <c r="O11">
@@ -1061,56 +1088,236 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="F12" s="2">
+        <v>800</v>
+      </c>
+      <c r="G12" s="2">
+        <v>43</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" ref="H12:H16" si="2">MROUND((D12/(E12*(F12/(PI()*G12))))*60,10)</f>
+        <v>110</v>
+      </c>
+      <c r="I12" s="2" cm="1">
+        <f t="array" ref="I12">_xlfn.IFS(C12="Milling",MROUND(350, 10), C12="Turning",MROUND(250, 10), C12="Drilling",MROUND(80, 10), C12="Grinding",MROUND(52, 10), C12="Boring",MROUND(88, 10), C12="Grooving",MROUND(230, 10), C12="Broaching",MROUND(220, 10), C12="Honing",MROUND(90, 10))</f>
+        <v>350</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="1"/>
+        <v>460</v>
+      </c>
       <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
+      <c r="L12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="N12" s="3"/>
+      <c r="O12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="1">
+        <v>70</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="F13" s="2">
+        <v>3800</v>
+      </c>
+      <c r="G13" s="2">
+        <v>50</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="2"/>
+        <v>390</v>
+      </c>
+      <c r="I13" s="2" cm="1">
+        <f t="array" ref="I13">_xlfn.IFS(C13="Milling",MROUND(350, 10), C13="Turning",MROUND(250, 10), C13="Drilling",MROUND(80, 10), C13="Grinding",MROUND(52, 10), C13="Boring",MROUND(88, 10), C13="Grooving",MROUND(230, 10), C13="Broaching",MROUND(220, 10), C13="Honing",MROUND(90, 10))</f>
+        <v>90</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="1"/>
+        <v>480</v>
+      </c>
       <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
+      <c r="L13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="N13" s="3"/>
+      <c r="O13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="1">
+        <v>45</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="F14" s="2">
+        <v>200</v>
+      </c>
+      <c r="G14" s="2">
+        <v>5</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="2"/>
+        <v>530</v>
+      </c>
+      <c r="I14" s="2" cm="1">
+        <f t="array" ref="I14">_xlfn.IFS(C14="Milling",MROUND(350, 10), C14="Turning",MROUND(250, 10), C14="Drilling",MROUND(80, 10), C14="Grinding",MROUND(52, 10), C14="Boring",MROUND(88, 10), C14="Grooving",MROUND(230, 10), C14="Broaching",MROUND(220, 10), C14="Honing",MROUND(90, 10))</f>
+        <v>230</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="1"/>
+        <v>760</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="N14" s="3"/>
+      <c r="O14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="F15" s="2">
+        <v>100</v>
+      </c>
+      <c r="G15" s="2">
+        <v>8</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="2"/>
+        <v>230</v>
+      </c>
+      <c r="I15" s="2" cm="1">
+        <f t="array" ref="I15">_xlfn.IFS(C15="Milling",MROUND(350, 10), C15="Turning",MROUND(250, 10), C15="Drilling",MROUND(80, 10), C15="Grinding",MROUND(52, 10), C15="Boring",MROUND(88, 10), C15="Grooving",MROUND(230, 10), C15="Broaching",MROUND(220, 10), C15="Honing",MROUND(90, 10))</f>
+        <v>90</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" si="1"/>
+        <v>320</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="L15" s="2"/>
+      <c r="M15" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="N15" s="3"/>
+      <c r="O15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="1">
+        <v>45</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="F16" s="2">
+        <v>3500</v>
+      </c>
+      <c r="G16" s="2">
+        <v>52</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="2"/>
+        <v>320</v>
+      </c>
+      <c r="I16" s="2" cm="1">
+        <f t="array" ref="I16">_xlfn.IFS(C16="Milling",MROUND(350, 10), C16="Turning",MROUND(250, 10), C16="Drilling",MROUND(80, 10), C16="Grinding",MROUND(52, 10), C16="Boring",MROUND(88, 10), C16="Grooving",MROUND(230, 10), C16="Broaching",MROUND(220, 10), C16="Honing",MROUND(90, 10))</f>
+        <v>80</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="L16" s="2"/>
+      <c r="M16" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="N16" s="3"/>
+      <c r="O16">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D17" s="2"/>

</xml_diff>